<commit_message>
Add battery voltage to escData plot
</commit_message>
<xml_diff>
--- a/CustomPlots/escData_Plot_Def.xlsx
+++ b/CustomPlots/escData_Plot_Def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3_bsp_ardupilot\CustomPlots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS\kVIS3_bsp_ardupilot\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8183B0-1927-4466-93D8-8A7BC8E67A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6BF84-868C-4944-BB0A-332AD102FE88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="52">
   <si>
     <t>KSID Custom Plot Definition</t>
   </si>
@@ -181,6 +184,12 @@
   </si>
   <si>
     <t>Current~[~A~]</t>
+  </si>
+  <si>
+    <t>BAT/Volt</t>
+  </si>
+  <si>
+    <t>BATT</t>
   </si>
 </sst>
 </file>
@@ -544,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7D595D-48C5-5044-8E94-F6ADF0970571}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1044,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18">
         <v>2</v>
@@ -1050,19 +1059,19 @@
         <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1088,13 +1097,13 @@
         <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1120,13 +1129,13 @@
         <v>24</v>
       </c>
       <c r="K20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
       <c r="R20" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1152,12 +1161,44 @@
         <v>24</v>
       </c>
       <c r="K21" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" t="s">
         <v>46</v>
       </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="R21" t="s">
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed for new file format
</commit_message>
<xml_diff>
--- a/CustomPlots/escData_Plot_Def.xlsx
+++ b/CustomPlots/escData_Plot_Def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS\kVIS3_bsp_ardupilot\CustomPlots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3\kVIS3_bsp_ardupilot\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6BF84-868C-4944-BB0A-332AD102FE88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1627204-F09C-455C-B292-E0969F4F1C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -114,18 +114,6 @@
     <t>escData</t>
   </si>
   <si>
-    <t>ESC1/RPM</t>
-  </si>
-  <si>
-    <t>ESC2/RPM</t>
-  </si>
-  <si>
-    <t>ESC3/RPM</t>
-  </si>
-  <si>
-    <t>ESC4/RPM</t>
-  </si>
-  <si>
     <t>RPM~[~1/s~]</t>
   </si>
   <si>
@@ -141,42 +129,6 @@
     <t>ESC2</t>
   </si>
   <si>
-    <t>ESC1/Temp</t>
-  </si>
-  <si>
-    <t>ESC3/Temp</t>
-  </si>
-  <si>
-    <t>ESC2/Temp</t>
-  </si>
-  <si>
-    <t>ESC4/Temp</t>
-  </si>
-  <si>
-    <t>ESC1/Volt</t>
-  </si>
-  <si>
-    <t>ESC2/Volt</t>
-  </si>
-  <si>
-    <t>ESC3/Volt</t>
-  </si>
-  <si>
-    <t>ESC4/Volt</t>
-  </si>
-  <si>
-    <t>ESC1/Curr</t>
-  </si>
-  <si>
-    <t>ESC2/Curr</t>
-  </si>
-  <si>
-    <t>ESC3/Curr</t>
-  </si>
-  <si>
-    <t>ESC4/Curr</t>
-  </si>
-  <si>
     <t>Temp~[~deg~]</t>
   </si>
   <si>
@@ -190,6 +142,54 @@
   </si>
   <si>
     <t>BATT</t>
+  </si>
+  <si>
+    <t>ESC_1/RPM</t>
+  </si>
+  <si>
+    <t>ESC_2/RPM</t>
+  </si>
+  <si>
+    <t>ESC_3/RPM</t>
+  </si>
+  <si>
+    <t>ESC_4/RPM</t>
+  </si>
+  <si>
+    <t>ESC_1/Temp</t>
+  </si>
+  <si>
+    <t>ESC_2/Temp</t>
+  </si>
+  <si>
+    <t>ESC_3/Temp</t>
+  </si>
+  <si>
+    <t>ESC_4/Temp</t>
+  </si>
+  <si>
+    <t>ESC_1/Volt</t>
+  </si>
+  <si>
+    <t>ESC_2/Volt</t>
+  </si>
+  <si>
+    <t>ESC_3/Volt</t>
+  </si>
+  <si>
+    <t>ESC_4/Volt</t>
+  </si>
+  <si>
+    <t>ESC_1/Curr</t>
+  </si>
+  <si>
+    <t>ESC_2/Curr</t>
+  </si>
+  <si>
+    <t>ESC_3/Curr</t>
+  </si>
+  <si>
+    <t>ESC_4/Curr</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -675,19 +675,19 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="R6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -707,19 +707,19 @@
         <v>23</v>
       </c>
       <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -739,19 +739,19 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
       </c>
       <c r="K8" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
         <v>28</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -771,19 +771,19 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
       </c>
       <c r="K9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
         <v>29</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -803,19 +803,19 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -835,19 +835,19 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="R11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -867,19 +867,19 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="O12">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -899,19 +899,19 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -931,19 +931,19 @@
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -963,19 +963,19 @@
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G15" t="s">
         <v>24</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="R15" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -995,19 +995,19 @@
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
       </c>
       <c r="K16" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="O16">
         <v>1</v>
       </c>
       <c r="R16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1027,19 +1027,19 @@
         <v>23</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G17" t="s">
         <v>24</v>
       </c>
       <c r="K17" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="O17">
         <v>1</v>
       </c>
       <c r="R17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1059,19 +1059,19 @@
         <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="G18" t="s">
         <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="O18">
         <v>1</v>
       </c>
       <c r="R18" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1091,19 +1091,19 @@
         <v>23</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G19" t="s">
         <v>24</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="O19">
         <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1123,19 +1123,19 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K20" t="s">
         <v>49</v>
       </c>
-      <c r="G20" t="s">
-        <v>24</v>
-      </c>
-      <c r="K20" t="s">
-        <v>44</v>
-      </c>
       <c r="O20">
         <v>1</v>
       </c>
       <c r="R20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1155,19 +1155,19 @@
         <v>23</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G21" t="s">
         <v>24</v>
       </c>
       <c r="K21" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="O21">
         <v>1</v>
       </c>
       <c r="R21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1187,19 +1187,19 @@
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G22" t="s">
         <v>24</v>
       </c>
       <c r="K22" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="O22">
         <v>1</v>
       </c>
       <c r="R22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>